<commit_message>
Added pricing and links of most components. Removed unneeded ones.
</commit_message>
<xml_diff>
--- a/projectManagement/components&costs.xlsx
+++ b/projectManagement/components&costs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\6. Semester\DT\dt-g5\projectManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NightPic\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB599868-25C4-4C93-BCD8-D527F9882DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_E3F5A9EDA04988343F3251EDC183AD4BD8BF5F3D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Bauteile:</t>
   </si>
@@ -44,37 +44,46 @@
     <t>Kosten:</t>
   </si>
   <si>
+    <t>Versand:</t>
+  </si>
+  <si>
+    <t>Gesamtkosten</t>
+  </si>
+  <si>
+    <t>Link:</t>
+  </si>
+  <si>
     <t>Mikrokontroller</t>
   </si>
   <si>
+    <t>rasppishop</t>
+  </si>
+  <si>
     <t>Kamera mit Infrarot</t>
   </si>
   <si>
-    <t>Infrarotsensor</t>
+    <t>buyzero</t>
   </si>
   <si>
     <t xml:space="preserve">Display </t>
   </si>
   <si>
-    <t>Mikrofon</t>
-  </si>
-  <si>
     <t>LED-Leuchten</t>
   </si>
   <si>
-    <t>Speicher</t>
-  </si>
-  <si>
-    <t>Netzteil</t>
+    <t>Spiegelfolie</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Glasscheibe</t>
+  </si>
+  <si>
+    <t>Gehäuse/Rahmen</t>
   </si>
   <si>
     <t>Verbindungskabel und Stecker</t>
-  </si>
-  <si>
-    <t>Gehäuse/Rahmen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spiegel </t>
   </si>
   <si>
     <t>Gesamt:</t>
@@ -87,10 +96,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,17 +139,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,125 +430,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>46.99</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="E2" s="2">
+        <f>SUM(C2,D2)</f>
+        <v>52.980000000000004</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>28.59</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="E3" s="2">
+        <f>SUM(C3,D3)</f>
+        <v>34.54</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E9" si="0">SUM(C4,D4)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>14.99</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>14.99</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>24.99</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>24.99</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
-        <v>10</v>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickTop="1">
+      <c r="A10" t="s">
+        <v>16</v>
       </c>
       <c r="C10" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2">
-        <f>SUM(C2:C12)</f>
-        <v>310</v>
+        <f>SUM(C2:C9)</f>
+        <v>115.55999999999999</v>
+      </c>
+      <c r="D10" s="2">
+        <f>SUM(D2:D9)</f>
+        <v>11.940000000000001</v>
+      </c>
+      <c r="E10" s="2">
+        <f>SUM(E2:E9)</f>
+        <v>127.5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>